<commit_message>
-Dodanie 2 plotów oraz widgetu dla plot2
-Dodanie plotu procentowego (plot 3)
-Dodanie plotu standardize scale (plot 4)
-Dodanie widgetu wyboru roku dla plot 2
</commit_message>
<xml_diff>
--- a/Szwajcaria Dane.xlsx
+++ b/Szwajcaria Dane.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>M.pop</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -53,12 +56,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -85,9 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -382,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -393,7 +406,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +437,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>37681</v>
       </c>
@@ -456,8 +472,11 @@
       <c r="J2">
         <v>3553058</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="2">
+        <v>6137000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>38047</v>
       </c>
@@ -488,8 +507,11 @@
       <c r="J3">
         <v>3578306</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="2">
+        <v>6235000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>38412</v>
       </c>
@@ -520,8 +542,11 @@
       <c r="J4">
         <v>3614707</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="2">
+        <v>6796000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>38777</v>
       </c>
@@ -552,8 +577,11 @@
       <c r="J5">
         <v>3647787</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="2">
+        <v>7388000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>39142</v>
       </c>
@@ -584,8 +612,11 @@
       <c r="J6">
         <v>3692432</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="2">
+        <v>8040000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>39508</v>
       </c>
@@ -616,8 +647,11 @@
       <c r="J7">
         <v>3740844</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="2">
+        <v>8683000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>39873</v>
       </c>
@@ -648,8 +682,11 @@
       <c r="J8">
         <v>3784429</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="2">
+        <v>9027000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>40238</v>
       </c>
@@ -680,8 +717,11 @@
       <c r="J9">
         <v>3829691</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="2">
+        <v>9414000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>40603</v>
       </c>
@@ -712,8 +752,11 @@
       <c r="J10">
         <v>3883940</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="2">
+        <v>9779000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>40969</v>
       </c>
@@ -744,8 +787,11 @@
       <c r="J11">
         <v>3931291</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="2">
+        <v>10028000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>41334</v>
       </c>
@@ -776,8 +822,11 @@
       <c r="J12">
         <v>3978842</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="2">
+        <v>10554000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>41699</v>
       </c>
@@ -808,8 +857,11 @@
       <c r="J13">
         <v>4033535</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="2">
+        <v>11938000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>42064</v>
       </c>
@@ -839,6 +891,9 @@
       </c>
       <c r="J14">
         <v>4077981</v>
+      </c>
+      <c r="K14" s="3">
+        <v>11933000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>